<commit_message>
report: results and conclusion updates (see #2)
</commit_message>
<xml_diff>
--- a/U2/report/testing.xlsx
+++ b/U2/report/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\SKOLA_CVUT\MGR\ADKG\U2\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100008_{F7607463-B060-4F2D-AD03-274921E290B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E29782E2-7A54-4E35-88CC-FA98FD064867}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{CEFAD511-70BF-4EA0-AF74-936C756BD128}"/>
   </bookViews>
@@ -306,15 +306,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -340,6 +331,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,34 +741,34 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92.6</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>539.29999999999995</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2091.6999999999998</c:v>
+                  <c:v>10.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4450.3999999999996</c:v>
+                  <c:v>16.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7818.6</c:v>
+                  <c:v>22.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31694.400000000001</c:v>
+                  <c:v>47.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>179290.2</c:v>
+                  <c:v>124.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>635048.4</c:v>
+                  <c:v>238.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2229,34 +2229,34 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.5</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.099999999999994</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>389.2</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1502.8</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3468.3</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6254.1</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25542</c:v>
+                  <c:v>14.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>185213.4</c:v>
+                  <c:v>38.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>799618.4</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2951,34 +2951,34 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.6</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84.4</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>462.9</c:v>
+                  <c:v>5.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1719.1</c:v>
+                  <c:v>10.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3723.1</c:v>
+                  <c:v>17.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6763.6</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27294.5</c:v>
+                  <c:v>43.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>179383.6</c:v>
+                  <c:v>103.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>745138.1</c:v>
+                  <c:v>186.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3720,34 +3720,34 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.5</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.099999999999994</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>389.2</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1502.8</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3468.3</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6254.1</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25542</c:v>
+                  <c:v>14.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>185213.4</c:v>
+                  <c:v>38.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>799618.4</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5208,34 +5208,34 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92.6</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>539.29999999999995</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2091.6999999999998</c:v>
+                  <c:v>10.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4450.3999999999996</c:v>
+                  <c:v>16.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7818.6</c:v>
+                  <c:v>22.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31694.400000000001</c:v>
+                  <c:v>47.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>179290.2</c:v>
+                  <c:v>124.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>635048.4</c:v>
+                  <c:v>238.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5373,7 +5373,6 @@
         <c:axId val="803222184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="800000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6651,34 +6650,34 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.6</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84.4</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>462.9</c:v>
+                  <c:v>5.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1719.1</c:v>
+                  <c:v>10.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3723.1</c:v>
+                  <c:v>17.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6763.6</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27294.5</c:v>
+                  <c:v>43.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>179383.6</c:v>
+                  <c:v>103.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>745138.1</c:v>
+                  <c:v>186.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14127,7 +14126,7 @@
   <dimension ref="B2:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14143,66 +14142,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="20"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="30"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="26" t="s">
+      <c r="G3" s="23"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="26"/>
-      <c r="K3" s="28"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="25"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="30"/>
-      <c r="C4" s="23" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="22" t="s">
         <v>6</v>
       </c>
     </row>
@@ -14220,9 +14219,9 @@
       </c>
       <c r="E5" s="6">
         <f>random!C46</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F5" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="18">
         <f>raster!$C$14</f>
         <v>25.7</v>
       </c>
@@ -14232,7 +14231,7 @@
       </c>
       <c r="H5" s="7">
         <f>raster!$C$46</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="I5" s="6">
         <f>circle!C14</f>
@@ -14244,7 +14243,7 @@
       </c>
       <c r="K5" s="7">
         <f>circle!C46</f>
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -14261,9 +14260,9 @@
       </c>
       <c r="E6" s="6">
         <f>random!D46</f>
-        <v>22.5</v>
-      </c>
-      <c r="F6" s="21">
+        <v>1</v>
+      </c>
+      <c r="F6" s="18">
         <f>raster!$D$14</f>
         <v>284.5</v>
       </c>
@@ -14273,7 +14272,7 @@
       </c>
       <c r="H6" s="7">
         <f>raster!$D$46</f>
-        <v>22.6</v>
+        <v>0.9</v>
       </c>
       <c r="I6" s="6">
         <f>circle!D14</f>
@@ -14285,7 +14284,7 @@
       </c>
       <c r="K6" s="7">
         <f>circle!D46</f>
-        <v>17.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -14302,9 +14301,9 @@
       </c>
       <c r="E7" s="6">
         <f>random!E46</f>
-        <v>92.6</v>
-      </c>
-      <c r="F7" s="21">
+        <v>2.1</v>
+      </c>
+      <c r="F7" s="18">
         <f>raster!$E$14</f>
         <v>794.2</v>
       </c>
@@ -14314,7 +14313,7 @@
       </c>
       <c r="H7" s="7">
         <f>raster!$E$46</f>
-        <v>84.4</v>
+        <v>2.1</v>
       </c>
       <c r="I7" s="6">
         <f>circle!E14</f>
@@ -14326,7 +14325,7 @@
       </c>
       <c r="K7" s="7">
         <f>circle!E46</f>
-        <v>71.099999999999994</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
@@ -14343,9 +14342,9 @@
       </c>
       <c r="E8" s="6">
         <f>random!F46</f>
-        <v>539.29999999999995</v>
-      </c>
-      <c r="F8" s="21">
+        <v>5.6</v>
+      </c>
+      <c r="F8" s="18">
         <f>raster!$F$14</f>
         <v>3207.6</v>
       </c>
@@ -14355,7 +14354,7 @@
       </c>
       <c r="H8" s="7">
         <f>raster!$F$46</f>
-        <v>462.9</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I8" s="6">
         <f>circle!F14</f>
@@ -14367,7 +14366,7 @@
       </c>
       <c r="K8" s="7">
         <f>circle!F46</f>
-        <v>389.2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
@@ -14384,9 +14383,9 @@
       </c>
       <c r="E9" s="6">
         <f>random!G46</f>
-        <v>2091.6999999999998</v>
-      </c>
-      <c r="F9" s="21">
+        <v>10.6</v>
+      </c>
+      <c r="F9" s="18">
         <f>raster!$G$14</f>
         <v>9096.5</v>
       </c>
@@ -14396,7 +14395,7 @@
       </c>
       <c r="H9" s="7">
         <f>raster!$G$46</f>
-        <v>1719.1</v>
+        <v>10.9</v>
       </c>
       <c r="I9" s="6">
         <f>circle!G14</f>
@@ -14408,7 +14407,7 @@
       </c>
       <c r="K9" s="7">
         <f>circle!G46</f>
-        <v>1502.8</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -14425,9 +14424,9 @@
       </c>
       <c r="E10" s="6">
         <f>random!H46</f>
-        <v>4450.3999999999996</v>
-      </c>
-      <c r="F10" s="21">
+        <v>16.2</v>
+      </c>
+      <c r="F10" s="18">
         <f>raster!$H$14</f>
         <v>16612.3</v>
       </c>
@@ -14437,7 +14436,7 @@
       </c>
       <c r="H10" s="7">
         <f>raster!$H$46</f>
-        <v>3723.1</v>
+        <v>17.2</v>
       </c>
       <c r="I10" s="6">
         <f>circle!H14</f>
@@ -14449,7 +14448,7 @@
       </c>
       <c r="K10" s="7">
         <f>circle!H46</f>
-        <v>3468.3</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
@@ -14466,9 +14465,9 @@
       </c>
       <c r="E11" s="6">
         <f>random!I46</f>
-        <v>7818.6</v>
-      </c>
-      <c r="F11" s="21">
+        <v>22.4</v>
+      </c>
+      <c r="F11" s="18">
         <f>raster!$I$14</f>
         <v>25434.799999999999</v>
       </c>
@@ -14478,7 +14477,7 @@
       </c>
       <c r="H11" s="7">
         <f>raster!$I$46</f>
-        <v>6763.6</v>
+        <v>22</v>
       </c>
       <c r="I11" s="6">
         <f>circle!I14</f>
@@ -14490,7 +14489,7 @@
       </c>
       <c r="K11" s="7">
         <f>circle!I46</f>
-        <v>6254.1</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -14507,9 +14506,9 @@
       </c>
       <c r="E12" s="6">
         <f>random!J46</f>
-        <v>31694.400000000001</v>
-      </c>
-      <c r="F12" s="21">
+        <v>47.3</v>
+      </c>
+      <c r="F12" s="18">
         <f>raster!$J$14</f>
         <v>71724</v>
       </c>
@@ -14519,7 +14518,7 @@
       </c>
       <c r="H12" s="7">
         <f>raster!$J$46</f>
-        <v>27294.5</v>
+        <v>43.9</v>
       </c>
       <c r="I12" s="6">
         <f>circle!J14</f>
@@ -14531,7 +14530,7 @@
       </c>
       <c r="K12" s="7">
         <f>circle!J46</f>
-        <v>25542</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
@@ -14548,9 +14547,9 @@
       </c>
       <c r="E13" s="6">
         <f>random!K46</f>
-        <v>179290.2</v>
-      </c>
-      <c r="F13" s="21">
+        <v>124.5</v>
+      </c>
+      <c r="F13" s="18">
         <f>raster!$K$14</f>
         <v>272534.8</v>
       </c>
@@ -14560,7 +14559,7 @@
       </c>
       <c r="H13" s="7">
         <f>raster!$K$46</f>
-        <v>179383.6</v>
+        <v>103.4</v>
       </c>
       <c r="I13" s="6">
         <f>circle!K14</f>
@@ -14572,7 +14571,7 @@
       </c>
       <c r="K13" s="7">
         <f>circle!K46</f>
-        <v>185213.4</v>
+        <v>38.700000000000003</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -14589,9 +14588,9 @@
       </c>
       <c r="E14" s="14">
         <f>random!L46</f>
-        <v>635048.4</v>
-      </c>
-      <c r="F14" s="22">
+        <v>238.9</v>
+      </c>
+      <c r="F14" s="19">
         <f>raster!$L$14</f>
         <v>567696.9</v>
       </c>
@@ -14601,7 +14600,7 @@
       </c>
       <c r="H14" s="15">
         <f>raster!$L$46</f>
-        <v>745138.1</v>
+        <v>186.3</v>
       </c>
       <c r="I14" s="14">
         <f>circle!L14</f>
@@ -14613,7 +14612,7 @@
       </c>
       <c r="K14" s="15">
         <f>circle!L46</f>
-        <v>799618.4</v>
+        <v>73.5</v>
       </c>
     </row>
   </sheetData>
@@ -14633,8 +14632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43718E85-AD71-4B48-9361-1429EADDF8C1}">
   <dimension ref="B2:M47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="V40" sqref="V40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14646,19 +14645,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="30"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -15136,19 +15135,19 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="20"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="30"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
@@ -15638,19 +15637,19 @@
       <c r="L32" s="3"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="20"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="30"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
@@ -15692,34 +15691,34 @@
         <v>1</v>
       </c>
       <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
         <v>1</v>
       </c>
-      <c r="D36" s="2">
-        <v>22</v>
-      </c>
       <c r="E36" s="2">
-        <v>87</v>
+        <v>3</v>
       </c>
       <c r="F36" s="2">
-        <v>556</v>
+        <v>5</v>
       </c>
       <c r="G36" s="2">
-        <v>2118</v>
+        <v>10</v>
       </c>
       <c r="H36" s="2">
-        <v>4459</v>
+        <v>17</v>
       </c>
       <c r="I36" s="2">
-        <v>7737</v>
+        <v>23</v>
       </c>
       <c r="J36" s="2">
-        <v>30720</v>
+        <v>45</v>
       </c>
       <c r="K36" s="2">
-        <v>179375</v>
+        <v>129</v>
       </c>
       <c r="L36" s="4">
-        <v>687846</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
@@ -15727,34 +15726,34 @@
         <v>2</v>
       </c>
       <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
         <v>1</v>
       </c>
-      <c r="D37" s="2">
+      <c r="E37" s="2">
+        <v>2</v>
+      </c>
+      <c r="F37" s="2">
+        <v>5</v>
+      </c>
+      <c r="G37" s="2">
+        <v>11</v>
+      </c>
+      <c r="H37" s="2">
+        <v>16</v>
+      </c>
+      <c r="I37" s="2">
         <v>22</v>
       </c>
-      <c r="E37" s="2">
-        <v>89</v>
-      </c>
-      <c r="F37" s="2">
-        <v>564</v>
-      </c>
-      <c r="G37" s="2">
-        <v>2056</v>
-      </c>
-      <c r="H37" s="2">
-        <v>4453</v>
-      </c>
-      <c r="I37" s="2">
-        <v>7729</v>
-      </c>
       <c r="J37" s="2">
-        <v>30366</v>
+        <v>46</v>
       </c>
       <c r="K37" s="2">
-        <v>183733</v>
+        <v>127</v>
       </c>
       <c r="L37" s="4">
-        <v>704175</v>
+        <v>260</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
@@ -15762,34 +15761,34 @@
         <v>3</v>
       </c>
       <c r="C38" s="2">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
         <v>1</v>
       </c>
-      <c r="D38" s="2">
+      <c r="E38" s="2">
+        <v>2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>6</v>
+      </c>
+      <c r="G38" s="2">
+        <v>11</v>
+      </c>
+      <c r="H38" s="2">
+        <v>16</v>
+      </c>
+      <c r="I38" s="2">
         <v>22</v>
       </c>
-      <c r="E38" s="2">
-        <v>92</v>
-      </c>
-      <c r="F38" s="2">
-        <v>554</v>
-      </c>
-      <c r="G38" s="2">
-        <v>2088</v>
-      </c>
-      <c r="H38" s="2">
-        <v>4445</v>
-      </c>
-      <c r="I38" s="2">
-        <v>7736</v>
-      </c>
       <c r="J38" s="2">
-        <v>30346</v>
+        <v>52</v>
       </c>
       <c r="K38" s="2">
-        <v>181597</v>
+        <v>129</v>
       </c>
       <c r="L38" s="4">
-        <v>654683</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
@@ -15797,34 +15796,34 @@
         <v>4</v>
       </c>
       <c r="C39" s="2">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
         <v>1</v>
       </c>
-      <c r="D39" s="2">
-        <v>22</v>
-      </c>
       <c r="E39" s="2">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="F39" s="2">
-        <v>540</v>
+        <v>6</v>
       </c>
       <c r="G39" s="2">
-        <v>2137</v>
+        <v>10</v>
       </c>
       <c r="H39" s="2">
-        <v>4478</v>
+        <v>17</v>
       </c>
       <c r="I39" s="2">
-        <v>7730</v>
+        <v>23</v>
       </c>
       <c r="J39" s="2">
-        <v>30396</v>
+        <v>46</v>
       </c>
       <c r="K39" s="2">
-        <v>177733</v>
+        <v>133</v>
       </c>
       <c r="L39" s="4">
-        <v>622306</v>
+        <v>273</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
@@ -15832,34 +15831,34 @@
         <v>5</v>
       </c>
       <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
         <v>1</v>
       </c>
-      <c r="D40" s="2">
-        <v>22</v>
-      </c>
       <c r="E40" s="2">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="F40" s="2">
-        <v>555</v>
+        <v>5</v>
       </c>
       <c r="G40" s="2">
-        <v>2082</v>
+        <v>10</v>
       </c>
       <c r="H40" s="2">
-        <v>4443</v>
+        <v>16</v>
       </c>
       <c r="I40" s="2">
-        <v>7758</v>
+        <v>23</v>
       </c>
       <c r="J40" s="2">
-        <v>34322</v>
+        <v>48</v>
       </c>
       <c r="K40" s="2">
-        <v>177403</v>
+        <v>133</v>
       </c>
       <c r="L40" s="4">
-        <v>617258</v>
+        <v>267</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
@@ -15867,34 +15866,34 @@
         <v>6</v>
       </c>
       <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2">
         <v>1</v>
       </c>
-      <c r="D41" s="2">
-        <v>22</v>
-      </c>
       <c r="E41" s="2">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="F41" s="2">
-        <v>531</v>
+        <v>6</v>
       </c>
       <c r="G41" s="2">
-        <v>2100</v>
+        <v>11</v>
       </c>
       <c r="H41" s="2">
-        <v>4442</v>
+        <v>16</v>
       </c>
       <c r="I41" s="2">
-        <v>7742</v>
+        <v>23</v>
       </c>
       <c r="J41" s="2">
-        <v>31732</v>
+        <v>46</v>
       </c>
       <c r="K41" s="2">
-        <v>177527</v>
+        <v>119</v>
       </c>
       <c r="L41" s="4">
-        <v>605910</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
@@ -15905,31 +15904,31 @@
         <v>1</v>
       </c>
       <c r="D42" s="2">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2">
+        <v>2</v>
+      </c>
+      <c r="F42" s="2">
+        <v>6</v>
+      </c>
+      <c r="G42" s="2">
+        <v>11</v>
+      </c>
+      <c r="H42" s="2">
+        <v>16</v>
+      </c>
+      <c r="I42" s="2">
         <v>22</v>
       </c>
-      <c r="E42" s="2">
-        <v>101</v>
-      </c>
-      <c r="F42" s="2">
-        <v>512</v>
-      </c>
-      <c r="G42" s="2">
-        <v>2018</v>
-      </c>
-      <c r="H42" s="2">
-        <v>4442</v>
-      </c>
-      <c r="I42" s="2">
-        <v>8107</v>
-      </c>
       <c r="J42" s="2">
-        <v>30937</v>
+        <v>47</v>
       </c>
       <c r="K42" s="2">
-        <v>179711</v>
+        <v>126</v>
       </c>
       <c r="L42" s="4">
-        <v>603503</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
@@ -15937,34 +15936,34 @@
         <v>8</v>
       </c>
       <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
         <v>1</v>
       </c>
-      <c r="D43" s="2">
-        <v>29</v>
-      </c>
       <c r="E43" s="2">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="F43" s="2">
-        <v>526</v>
+        <v>5</v>
       </c>
       <c r="G43" s="2">
-        <v>2160</v>
+        <v>10</v>
       </c>
       <c r="H43" s="2">
-        <v>4442</v>
+        <v>16</v>
       </c>
       <c r="I43" s="2">
-        <v>8137</v>
+        <v>22</v>
       </c>
       <c r="J43" s="2">
-        <v>31894</v>
+        <v>46</v>
       </c>
       <c r="K43" s="2">
-        <v>175928</v>
+        <v>115</v>
       </c>
       <c r="L43" s="4">
-        <v>616161</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
@@ -15972,34 +15971,34 @@
         <v>9</v>
       </c>
       <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2">
         <v>2</v>
       </c>
-      <c r="D44" s="2">
+      <c r="F44" s="2">
+        <v>6</v>
+      </c>
+      <c r="G44" s="2">
+        <v>11</v>
+      </c>
+      <c r="H44" s="2">
+        <v>16</v>
+      </c>
+      <c r="I44" s="2">
         <v>21</v>
       </c>
-      <c r="E44" s="2">
-        <v>90</v>
-      </c>
-      <c r="F44" s="2">
-        <v>529</v>
-      </c>
-      <c r="G44" s="2">
-        <v>2048</v>
-      </c>
-      <c r="H44" s="2">
-        <v>4456</v>
-      </c>
-      <c r="I44" s="2">
-        <v>7730</v>
-      </c>
       <c r="J44" s="2">
-        <v>32097</v>
+        <v>51</v>
       </c>
       <c r="K44" s="2">
-        <v>181377</v>
+        <v>117</v>
       </c>
       <c r="L44" s="4">
-        <v>623966</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
@@ -16007,34 +16006,34 @@
         <v>10</v>
       </c>
       <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1">
         <v>1</v>
       </c>
-      <c r="D45" s="1">
-        <v>21</v>
-      </c>
       <c r="E45" s="1">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="F45" s="1">
-        <v>526</v>
+        <v>6</v>
       </c>
       <c r="G45" s="1">
-        <v>2110</v>
+        <v>11</v>
       </c>
       <c r="H45" s="1">
-        <v>4444</v>
+        <v>16</v>
       </c>
       <c r="I45" s="1">
-        <v>7780</v>
+        <v>23</v>
       </c>
       <c r="J45" s="1">
-        <v>34134</v>
+        <v>46</v>
       </c>
       <c r="K45" s="1">
-        <v>178518</v>
+        <v>117</v>
       </c>
       <c r="L45" s="5">
-        <v>614676</v>
+        <v>217</v>
       </c>
       <c r="M45" s="2"/>
     </row>
@@ -16044,43 +16043,43 @@
       </c>
       <c r="C46" s="16">
         <f>AVERAGE(C36:C45)</f>
-        <v>1.1000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="D46" s="16">
         <f>AVERAGE(D36:D45)</f>
-        <v>22.5</v>
+        <v>1</v>
       </c>
       <c r="E46" s="16">
         <f>AVERAGE(E36:E45)</f>
-        <v>92.6</v>
+        <v>2.1</v>
       </c>
       <c r="F46" s="16">
         <f>AVERAGE(F36:F45)</f>
-        <v>539.29999999999995</v>
+        <v>5.6</v>
       </c>
       <c r="G46" s="16">
         <f t="shared" ref="G46:L46" si="4">AVERAGE(G36:G45)</f>
-        <v>2091.6999999999998</v>
+        <v>10.6</v>
       </c>
       <c r="H46" s="16">
         <f t="shared" si="4"/>
-        <v>4450.3999999999996</v>
+        <v>16.2</v>
       </c>
       <c r="I46" s="16">
         <f t="shared" si="4"/>
-        <v>7818.6</v>
+        <v>22.4</v>
       </c>
       <c r="J46" s="16">
         <f t="shared" si="4"/>
-        <v>31694.400000000001</v>
+        <v>47.3</v>
       </c>
       <c r="K46" s="16">
         <f t="shared" si="4"/>
-        <v>179290.2</v>
+        <v>124.5</v>
       </c>
       <c r="L46" s="17">
         <f t="shared" si="4"/>
-        <v>635048.4</v>
+        <v>238.9</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
@@ -16093,39 +16092,39 @@
       </c>
       <c r="D47" s="1">
         <f>_xlfn.VAR.P(D36:D45)</f>
-        <v>4.8499999999999996</v>
+        <v>0</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" ref="E47:L47" si="5">_xlfn.VAR.P(E36:E45)</f>
-        <v>37.040000000000006</v>
+        <v>0.09</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="5"/>
-        <v>262.61</v>
+        <v>0.24</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="5"/>
-        <v>1653.61</v>
+        <v>0.24</v>
       </c>
       <c r="H47" s="1">
         <f t="shared" si="5"/>
-        <v>121.03999999999999</v>
+        <v>0.16000000000000006</v>
       </c>
       <c r="I47" s="1">
         <f t="shared" si="5"/>
-        <v>23279.24</v>
+        <v>0.44000000000000006</v>
       </c>
       <c r="J47" s="1">
         <f t="shared" si="5"/>
-        <v>1985105.2399999998</v>
+        <v>5.01</v>
       </c>
       <c r="K47" s="1">
         <f t="shared" si="5"/>
-        <v>5059474.76</v>
+        <v>42.65</v>
       </c>
       <c r="L47" s="5">
         <f t="shared" si="5"/>
-        <v>1116920476.6399999</v>
+        <v>503.69000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -16144,8 +16143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA39256-3695-4672-B35F-390AEC96F2C8}">
   <dimension ref="B2:L47"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView topLeftCell="E34" workbookViewId="0">
+      <selection activeCell="Q56" sqref="Q56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16156,19 +16155,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="30"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -16658,19 +16657,19 @@
       <c r="L16" s="3"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="20"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="30"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
@@ -17148,19 +17147,19 @@
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="20"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="30"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
@@ -17202,34 +17201,34 @@
         <v>1</v>
       </c>
       <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
         <v>1</v>
       </c>
-      <c r="D36" s="2">
-        <v>18</v>
-      </c>
       <c r="E36" s="2">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="F36" s="2">
-        <v>513</v>
+        <v>5</v>
       </c>
       <c r="G36" s="2">
-        <v>1949</v>
+        <v>11</v>
       </c>
       <c r="H36" s="2">
-        <v>3953</v>
+        <v>19</v>
       </c>
       <c r="I36" s="2">
-        <v>6979</v>
+        <v>21</v>
       </c>
       <c r="J36" s="2">
-        <v>27301</v>
+        <v>44</v>
       </c>
       <c r="K36" s="2">
-        <v>185474</v>
+        <v>103</v>
       </c>
       <c r="L36" s="4">
-        <v>731112</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
@@ -17240,31 +17239,31 @@
         <v>1</v>
       </c>
       <c r="D37" s="2">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E37" s="2">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="F37" s="2">
-        <v>540</v>
+        <v>5</v>
       </c>
       <c r="G37" s="2">
-        <v>1659</v>
+        <v>11</v>
       </c>
       <c r="H37" s="2">
-        <v>3702</v>
+        <v>17</v>
       </c>
       <c r="I37" s="2">
-        <v>6926</v>
+        <v>20</v>
       </c>
       <c r="J37" s="2">
-        <v>28434</v>
+        <v>44</v>
       </c>
       <c r="K37" s="2">
-        <v>192066</v>
+        <v>104</v>
       </c>
       <c r="L37" s="4">
-        <v>734554</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
@@ -17272,34 +17271,34 @@
         <v>3</v>
       </c>
       <c r="C38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="2">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E38" s="2">
+        <v>2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>6</v>
+      </c>
+      <c r="G38" s="2">
+        <v>11</v>
+      </c>
+      <c r="H38" s="2">
+        <v>15</v>
+      </c>
+      <c r="I38" s="2">
+        <v>20</v>
+      </c>
+      <c r="J38" s="2">
+        <v>48</v>
+      </c>
+      <c r="K38" s="2">
         <v>103</v>
       </c>
-      <c r="F38" s="2">
-        <v>481</v>
-      </c>
-      <c r="G38" s="2">
-        <v>1680</v>
-      </c>
-      <c r="H38" s="2">
-        <v>3639</v>
-      </c>
-      <c r="I38" s="2">
-        <v>6815</v>
-      </c>
-      <c r="J38" s="2">
-        <v>26853</v>
-      </c>
-      <c r="K38" s="2">
-        <v>172465</v>
-      </c>
       <c r="L38" s="4">
-        <v>738494</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
@@ -17307,34 +17306,34 @@
         <v>4</v>
       </c>
       <c r="C39" s="2">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
         <v>1</v>
       </c>
-      <c r="D39" s="2">
-        <v>30</v>
-      </c>
       <c r="E39" s="2">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="F39" s="2">
-        <v>413</v>
+        <v>5</v>
       </c>
       <c r="G39" s="2">
-        <v>1682</v>
+        <v>10</v>
       </c>
       <c r="H39" s="2">
-        <v>3653</v>
+        <v>17</v>
       </c>
       <c r="I39" s="2">
-        <v>6761</v>
+        <v>21</v>
       </c>
       <c r="J39" s="2">
-        <v>26476</v>
+        <v>43</v>
       </c>
       <c r="K39" s="2">
-        <v>172697</v>
+        <v>103</v>
       </c>
       <c r="L39" s="4">
-        <v>766781</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
@@ -17342,34 +17341,34 @@
         <v>5</v>
       </c>
       <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
         <v>1</v>
       </c>
-      <c r="D40" s="2">
-        <v>27</v>
-      </c>
       <c r="E40" s="2">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="F40" s="2">
-        <v>441</v>
+        <v>5</v>
       </c>
       <c r="G40" s="2">
-        <v>1711</v>
+        <v>11</v>
       </c>
       <c r="H40" s="2">
-        <v>3772</v>
+        <v>16</v>
       </c>
       <c r="I40" s="2">
-        <v>6787</v>
+        <v>28</v>
       </c>
       <c r="J40" s="2">
-        <v>26998</v>
+        <v>43</v>
       </c>
       <c r="K40" s="2">
-        <v>176790</v>
+        <v>103</v>
       </c>
       <c r="L40" s="4">
-        <v>740781</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
@@ -17377,34 +17376,34 @@
         <v>6</v>
       </c>
       <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2">
         <v>1</v>
       </c>
-      <c r="D41" s="2">
-        <v>25</v>
-      </c>
       <c r="E41" s="2">
-        <v>87</v>
+        <v>3</v>
       </c>
       <c r="F41" s="2">
-        <v>476</v>
+        <v>5</v>
       </c>
       <c r="G41" s="2">
-        <v>1692</v>
+        <v>11</v>
       </c>
       <c r="H41" s="2">
-        <v>3787</v>
+        <v>17</v>
       </c>
       <c r="I41" s="2">
-        <v>6616</v>
+        <v>21</v>
       </c>
       <c r="J41" s="2">
-        <v>26880</v>
+        <v>42</v>
       </c>
       <c r="K41" s="2">
-        <v>173146</v>
+        <v>103</v>
       </c>
       <c r="L41" s="4">
-        <v>744832</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
@@ -17412,34 +17411,34 @@
         <v>7</v>
       </c>
       <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2">
         <v>1</v>
       </c>
-      <c r="D42" s="2">
-        <v>28</v>
-      </c>
       <c r="E42" s="2">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="F42" s="2">
-        <v>439</v>
+        <v>5</v>
       </c>
       <c r="G42" s="2">
-        <v>1679</v>
+        <v>11</v>
       </c>
       <c r="H42" s="2">
-        <v>3766</v>
+        <v>22</v>
       </c>
       <c r="I42" s="2">
-        <v>6652</v>
+        <v>21</v>
       </c>
       <c r="J42" s="2">
-        <v>26601</v>
+        <v>45</v>
       </c>
       <c r="K42" s="2">
-        <v>174392</v>
+        <v>102</v>
       </c>
       <c r="L42" s="4">
-        <v>748824</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
@@ -17447,34 +17446,34 @@
         <v>8</v>
       </c>
       <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
         <v>1</v>
       </c>
-      <c r="D43" s="2">
-        <v>25</v>
-      </c>
       <c r="E43" s="2">
-        <v>83</v>
+        <v>2</v>
       </c>
       <c r="F43" s="2">
-        <v>443</v>
+        <v>5</v>
       </c>
       <c r="G43" s="2">
-        <v>1684</v>
+        <v>11</v>
       </c>
       <c r="H43" s="2">
-        <v>3639</v>
+        <v>17</v>
       </c>
       <c r="I43" s="2">
-        <v>6772</v>
+        <v>21</v>
       </c>
       <c r="J43" s="2">
-        <v>28396</v>
+        <v>42</v>
       </c>
       <c r="K43" s="2">
-        <v>174975</v>
+        <v>107</v>
       </c>
       <c r="L43" s="4">
-        <v>748654</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
@@ -17482,34 +17481,34 @@
         <v>9</v>
       </c>
       <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2">
         <v>1</v>
       </c>
-      <c r="D44" s="2">
-        <v>18</v>
-      </c>
       <c r="E44" s="2">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="F44" s="2">
-        <v>449</v>
+        <v>5</v>
       </c>
       <c r="G44" s="2">
-        <v>1771</v>
+        <v>11</v>
       </c>
       <c r="H44" s="2">
-        <v>3648</v>
+        <v>16</v>
       </c>
       <c r="I44" s="2">
-        <v>6595</v>
+        <v>21</v>
       </c>
       <c r="J44" s="2">
-        <v>27619</v>
+        <v>43</v>
       </c>
       <c r="K44" s="2">
-        <v>177023</v>
+        <v>103</v>
       </c>
       <c r="L44" s="4">
-        <v>749009</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
@@ -17517,34 +17516,34 @@
         <v>10</v>
       </c>
       <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1">
         <v>1</v>
       </c>
-      <c r="D45" s="1">
-        <v>18</v>
-      </c>
       <c r="E45" s="1">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="F45" s="1">
-        <v>434</v>
+        <v>5</v>
       </c>
       <c r="G45" s="1">
-        <v>1684</v>
+        <v>11</v>
       </c>
       <c r="H45" s="1">
-        <v>3672</v>
+        <v>16</v>
       </c>
       <c r="I45" s="1">
-        <v>6733</v>
+        <v>26</v>
       </c>
       <c r="J45" s="1">
-        <v>27387</v>
+        <v>45</v>
       </c>
       <c r="K45" s="1">
-        <v>194808</v>
+        <v>103</v>
       </c>
       <c r="L45" s="5">
-        <v>748340</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
@@ -17553,43 +17552,43 @@
       </c>
       <c r="C46" s="16">
         <f>AVERAGE(C36:C45)</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D46" s="16">
         <f>AVERAGE(D36:D45)</f>
-        <v>22.6</v>
+        <v>0.9</v>
       </c>
       <c r="E46" s="16">
         <f>AVERAGE(E36:E45)</f>
-        <v>84.4</v>
+        <v>2.1</v>
       </c>
       <c r="F46" s="16">
         <f t="shared" ref="F46:L46" si="4">AVERAGE(F36:F45)</f>
-        <v>462.9</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G46" s="16">
         <f t="shared" si="4"/>
-        <v>1719.1</v>
+        <v>10.9</v>
       </c>
       <c r="H46" s="16">
         <f t="shared" si="4"/>
-        <v>3723.1</v>
+        <v>17.2</v>
       </c>
       <c r="I46" s="16">
         <f t="shared" si="4"/>
-        <v>6763.6</v>
+        <v>22</v>
       </c>
       <c r="J46" s="16">
         <f t="shared" si="4"/>
-        <v>27294.5</v>
+        <v>43.9</v>
       </c>
       <c r="K46" s="16">
         <f t="shared" si="4"/>
-        <v>179383.6</v>
+        <v>103.4</v>
       </c>
       <c r="L46" s="17">
         <f t="shared" si="4"/>
-        <v>745138.1</v>
+        <v>186.3</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
@@ -17598,43 +17597,43 @@
       </c>
       <c r="C47" s="1">
         <f>_xlfn.VAR.P(C36:C45)</f>
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="D47" s="1">
         <f>_xlfn.VAR.P(D36:D45)</f>
-        <v>21.24</v>
+        <v>0.09</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" ref="E47:K47" si="5">_xlfn.VAR.P(E36:E45)</f>
-        <v>142.04</v>
+        <v>0.09</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="5"/>
-        <v>1391.8899999999999</v>
+        <v>8.9999999999999983E-2</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="5"/>
-        <v>6693.6900000000005</v>
+        <v>8.9999999999999983E-2</v>
       </c>
       <c r="H47" s="1">
         <f t="shared" si="5"/>
-        <v>8892.489999999998</v>
+        <v>3.56</v>
       </c>
       <c r="I47" s="1">
         <f t="shared" si="5"/>
-        <v>13964.039999999999</v>
+        <v>6.6</v>
       </c>
       <c r="J47" s="1">
         <f t="shared" si="5"/>
-        <v>423119.05</v>
+        <v>2.890000000000001</v>
       </c>
       <c r="K47" s="1">
         <f t="shared" si="5"/>
-        <v>62398467.439999998</v>
+        <v>1.64</v>
       </c>
       <c r="L47" s="5">
         <f>_xlfn.VAR.P(L36:L45)</f>
-        <v>89157529.890000015</v>
+        <v>8.6099999999999977</v>
       </c>
     </row>
   </sheetData>
@@ -17653,8 +17652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CA9B0B-6E4A-4DC5-8A5C-4BD9F8C6BE37}">
   <dimension ref="B2:L47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="W42" sqref="W42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17665,19 +17664,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="30"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
@@ -18155,19 +18154,19 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="20"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="30"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
@@ -18658,19 +18657,19 @@
       <c r="L32" s="6"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="20"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="30"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
@@ -18712,34 +18711,34 @@
         <v>1</v>
       </c>
       <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
         <v>1</v>
       </c>
-      <c r="D36" s="2">
-        <v>18</v>
-      </c>
       <c r="E36" s="2">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="F36" s="2">
-        <v>384</v>
+        <v>2</v>
       </c>
       <c r="G36" s="2">
-        <v>1538</v>
+        <v>4</v>
       </c>
       <c r="H36" s="2">
-        <v>3749</v>
+        <v>6</v>
       </c>
       <c r="I36" s="2">
-        <v>6155</v>
+        <v>8</v>
       </c>
       <c r="J36" s="2">
-        <v>25488</v>
+        <v>15</v>
       </c>
       <c r="K36" s="2">
-        <v>177410</v>
+        <v>37</v>
       </c>
       <c r="L36" s="4">
-        <v>800141</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
@@ -18750,31 +18749,31 @@
         <v>1</v>
       </c>
       <c r="D37" s="2">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E37" s="2">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="F37" s="2">
-        <v>417</v>
+        <v>2</v>
       </c>
       <c r="G37" s="2">
-        <v>1509</v>
+        <v>4</v>
       </c>
       <c r="H37" s="2">
-        <v>3432</v>
+        <v>6</v>
       </c>
       <c r="I37" s="2">
-        <v>6149</v>
+        <v>7</v>
       </c>
       <c r="J37" s="2">
-        <v>25163</v>
+        <v>14</v>
       </c>
       <c r="K37" s="2">
-        <v>177432</v>
+        <v>36</v>
       </c>
       <c r="L37" s="4">
-        <v>778327</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
@@ -18782,34 +18781,34 @@
         <v>3</v>
       </c>
       <c r="C38" s="2">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
         <v>1</v>
       </c>
-      <c r="D38" s="2">
-        <v>17</v>
-      </c>
       <c r="E38" s="2">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="F38" s="2">
-        <v>409</v>
+        <v>3</v>
       </c>
       <c r="G38" s="2">
-        <v>1489</v>
+        <v>4</v>
       </c>
       <c r="H38" s="2">
-        <v>3442</v>
+        <v>6</v>
       </c>
       <c r="I38" s="2">
-        <v>6192</v>
+        <v>8</v>
       </c>
       <c r="J38" s="2">
-        <v>25118</v>
+        <v>14</v>
       </c>
       <c r="K38" s="2">
-        <v>177524</v>
+        <v>52</v>
       </c>
       <c r="L38" s="4">
-        <v>783551</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
@@ -18817,34 +18816,34 @@
         <v>4</v>
       </c>
       <c r="C39" s="2">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
         <v>1</v>
       </c>
-      <c r="D39" s="2">
-        <v>18</v>
-      </c>
       <c r="E39" s="2">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="F39" s="2">
-        <v>403</v>
+        <v>2</v>
       </c>
       <c r="G39" s="2">
-        <v>1500</v>
+        <v>4</v>
       </c>
       <c r="H39" s="2">
-        <v>3434</v>
+        <v>6</v>
       </c>
       <c r="I39" s="2">
-        <v>6143</v>
+        <v>8</v>
       </c>
       <c r="J39" s="2">
-        <v>25055</v>
+        <v>14</v>
       </c>
       <c r="K39" s="2">
-        <v>179082</v>
+        <v>36</v>
       </c>
       <c r="L39" s="4">
-        <v>811857</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
@@ -18852,34 +18851,34 @@
         <v>5</v>
       </c>
       <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
         <v>1</v>
       </c>
-      <c r="D40" s="2">
-        <v>17</v>
-      </c>
       <c r="E40" s="2">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="F40" s="2">
-        <v>393</v>
+        <v>2</v>
       </c>
       <c r="G40" s="2">
-        <v>1499</v>
+        <v>4</v>
       </c>
       <c r="H40" s="2">
-        <v>3451</v>
+        <v>6</v>
       </c>
       <c r="I40" s="2">
-        <v>6149</v>
+        <v>8</v>
       </c>
       <c r="J40" s="2">
-        <v>25164</v>
+        <v>14</v>
       </c>
       <c r="K40" s="2">
-        <v>181440</v>
+        <v>35</v>
       </c>
       <c r="L40" s="4">
-        <v>790292</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
@@ -18887,34 +18886,34 @@
         <v>6</v>
       </c>
       <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2">
         <v>1</v>
       </c>
-      <c r="D41" s="2">
-        <v>18</v>
-      </c>
-      <c r="E41" s="2">
-        <v>63</v>
-      </c>
       <c r="F41" s="2">
-        <v>375</v>
+        <v>4</v>
       </c>
       <c r="G41" s="2">
-        <v>1497</v>
+        <v>4</v>
       </c>
       <c r="H41" s="2">
-        <v>3434</v>
+        <v>6</v>
       </c>
       <c r="I41" s="2">
-        <v>6556</v>
+        <v>7</v>
       </c>
       <c r="J41" s="2">
-        <v>25038</v>
+        <v>14</v>
       </c>
       <c r="K41" s="2">
-        <v>183571</v>
+        <v>39</v>
       </c>
       <c r="L41" s="4">
-        <v>789612</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
@@ -18922,34 +18921,34 @@
         <v>7</v>
       </c>
       <c r="C42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" s="2">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E42" s="2">
-        <v>79</v>
+        <v>2</v>
       </c>
       <c r="F42" s="2">
-        <v>388</v>
+        <v>3</v>
       </c>
       <c r="G42" s="2">
-        <v>1497</v>
+        <v>5</v>
       </c>
       <c r="H42" s="2">
-        <v>3434</v>
+        <v>6</v>
       </c>
       <c r="I42" s="2">
-        <v>6344</v>
+        <v>8</v>
       </c>
       <c r="J42" s="2">
-        <v>25667</v>
+        <v>14</v>
       </c>
       <c r="K42" s="2">
-        <v>181185</v>
+        <v>36</v>
       </c>
       <c r="L42" s="4">
-        <v>798544</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
@@ -18960,31 +18959,31 @@
         <v>1</v>
       </c>
       <c r="D43" s="2">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E43" s="2">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="F43" s="2">
-        <v>373</v>
+        <v>2</v>
       </c>
       <c r="G43" s="2">
-        <v>1496</v>
+        <v>5</v>
       </c>
       <c r="H43" s="2">
-        <v>3436</v>
+        <v>5</v>
       </c>
       <c r="I43" s="2">
-        <v>6383</v>
+        <v>8</v>
       </c>
       <c r="J43" s="2">
-        <v>25173</v>
+        <v>14</v>
       </c>
       <c r="K43" s="2">
-        <v>212314</v>
+        <v>43</v>
       </c>
       <c r="L43" s="4">
-        <v>799568</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
@@ -18992,34 +18991,34 @@
         <v>9</v>
       </c>
       <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2">
         <v>1</v>
       </c>
-      <c r="D44" s="2">
-        <v>18</v>
-      </c>
       <c r="E44" s="2">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="F44" s="2">
-        <v>379</v>
+        <v>2</v>
       </c>
       <c r="G44" s="2">
-        <v>1503</v>
+        <v>4</v>
       </c>
       <c r="H44" s="2">
-        <v>3433</v>
+        <v>6</v>
       </c>
       <c r="I44" s="2">
-        <v>6315</v>
+        <v>7</v>
       </c>
       <c r="J44" s="2">
-        <v>25132</v>
+        <v>14</v>
       </c>
       <c r="K44" s="2">
-        <v>194856</v>
+        <v>36</v>
       </c>
       <c r="L44" s="4">
-        <v>825592</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
@@ -19027,34 +19026,34 @@
         <v>10</v>
       </c>
       <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1">
         <v>1</v>
       </c>
-      <c r="D45" s="1">
-        <v>17</v>
-      </c>
       <c r="E45" s="1">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="F45" s="1">
-        <v>371</v>
+        <v>3</v>
       </c>
       <c r="G45" s="1">
-        <v>1500</v>
+        <v>4</v>
       </c>
       <c r="H45" s="1">
-        <v>3438</v>
+        <v>5</v>
       </c>
       <c r="I45" s="1">
-        <v>6155</v>
+        <v>7</v>
       </c>
       <c r="J45" s="1">
-        <v>28422</v>
+        <v>14</v>
       </c>
       <c r="K45" s="1">
-        <v>187320</v>
+        <v>37</v>
       </c>
       <c r="L45" s="5">
-        <v>818700</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
@@ -19063,43 +19062,43 @@
       </c>
       <c r="C46" s="16">
         <f>AVERAGE(C36:C45)</f>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="D46" s="16">
         <f>AVERAGE(D36:D45)</f>
-        <v>17.5</v>
+        <v>0.8</v>
       </c>
       <c r="E46" s="16">
         <f>AVERAGE(E36:E45)</f>
-        <v>71.099999999999994</v>
+        <v>1.4</v>
       </c>
       <c r="F46" s="16">
         <f t="shared" ref="F46:L46" si="4">AVERAGE(F36:F45)</f>
-        <v>389.2</v>
+        <v>2.5</v>
       </c>
       <c r="G46" s="16">
         <f t="shared" si="4"/>
-        <v>1502.8</v>
+        <v>4.2</v>
       </c>
       <c r="H46" s="16">
         <f t="shared" si="4"/>
-        <v>3468.3</v>
+        <v>5.8</v>
       </c>
       <c r="I46" s="16">
         <f t="shared" si="4"/>
-        <v>6254.1</v>
+        <v>7.6</v>
       </c>
       <c r="J46" s="16">
         <f t="shared" si="4"/>
-        <v>25542</v>
+        <v>14.1</v>
       </c>
       <c r="K46" s="16">
         <f t="shared" si="4"/>
-        <v>185213.4</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="L46" s="17">
         <f t="shared" si="4"/>
-        <v>799618.4</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
@@ -19108,43 +19107,43 @@
       </c>
       <c r="C47" s="1">
         <f>_xlfn.VAR.P(C36:C45)</f>
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="D47" s="1">
         <f>_xlfn.VAR.P(D36:D45)</f>
-        <v>0.25</v>
+        <v>0.16</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" ref="E47:L47" si="5">_xlfn.VAR.P(E36:E45)</f>
-        <v>54.09</v>
+        <v>0.24</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="5"/>
-        <v>229.76</v>
+        <v>0.45</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="5"/>
-        <v>161.15999999999994</v>
+        <v>0.15999999999999998</v>
       </c>
       <c r="H47" s="1">
         <f t="shared" si="5"/>
-        <v>8783.8100000000031</v>
+        <v>0.15999999999999998</v>
       </c>
       <c r="I47" s="1">
         <f t="shared" si="5"/>
-        <v>17748.29</v>
+        <v>0.24</v>
       </c>
       <c r="J47" s="1">
         <f t="shared" si="5"/>
-        <v>957468.8</v>
+        <v>8.9999999999999969E-2</v>
       </c>
       <c r="K47" s="1">
         <f t="shared" si="5"/>
-        <v>108318822.64000002</v>
+        <v>24.41</v>
       </c>
       <c r="L47" s="5">
         <f t="shared" si="5"/>
-        <v>208854350.64000002</v>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>